<commit_message>
moved postgres manager object initialization to loader.py
added "Завершить общение" button for client side while consulting with consultant.
</commit_message>
<xml_diff>
--- a/data/database_backup/logs.xlsx
+++ b/data/database_backup/logs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E206"/>
+  <dimension ref="A1:E215"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4760,6 +4760,195 @@
         </is>
       </c>
     </row>
+    <row r="207">
+      <c r="A207" s="1" t="n">
+        <v>205</v>
+      </c>
+      <c r="B207" t="n">
+        <v>206</v>
+      </c>
+      <c r="C207" t="n">
+        <v>3</v>
+      </c>
+      <c r="D207" t="inlineStr">
+        <is>
+          <t>Начал взаимодействие с консультантом!</t>
+        </is>
+      </c>
+      <c r="E207" t="inlineStr">
+        <is>
+          <t>09/06/2023 17:50:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" s="1" t="n">
+        <v>206</v>
+      </c>
+      <c r="B208" t="n">
+        <v>207</v>
+      </c>
+      <c r="C208" t="n">
+        <v>5</v>
+      </c>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t>Успешно добавлен в базу!</t>
+        </is>
+      </c>
+      <c r="E208" t="inlineStr">
+        <is>
+          <t>09/06/2023 18:11:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" s="1" t="n">
+        <v>207</v>
+      </c>
+      <c r="B209" t="n">
+        <v>208</v>
+      </c>
+      <c r="C209" t="n">
+        <v>5</v>
+      </c>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>Начал взаимодействие с консультантом!</t>
+        </is>
+      </c>
+      <c r="E209" t="inlineStr">
+        <is>
+          <t>09/06/2023 18:11:18</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" s="1" t="n">
+        <v>208</v>
+      </c>
+      <c r="B210" t="n">
+        <v>209</v>
+      </c>
+      <c r="C210" t="n">
+        <v>1</v>
+      </c>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>Начал взаимодействие с консультантом!</t>
+        </is>
+      </c>
+      <c r="E210" t="inlineStr">
+        <is>
+          <t>11/06/2023 21:33:25</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" s="1" t="n">
+        <v>209</v>
+      </c>
+      <c r="B211" t="n">
+        <v>210</v>
+      </c>
+      <c r="C211" t="n">
+        <v>1</v>
+      </c>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>Начал взаимодействие с консультантом!</t>
+        </is>
+      </c>
+      <c r="E211" t="inlineStr">
+        <is>
+          <t>11/06/2023 23:11:18</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" s="1" t="n">
+        <v>210</v>
+      </c>
+      <c r="B212" t="n">
+        <v>211</v>
+      </c>
+      <c r="C212" t="n">
+        <v>1</v>
+      </c>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>Начал взаимодействие с консультантом!</t>
+        </is>
+      </c>
+      <c r="E212" t="inlineStr">
+        <is>
+          <t>11/06/2023 23:17:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" s="1" t="n">
+        <v>211</v>
+      </c>
+      <c r="B213" t="n">
+        <v>212</v>
+      </c>
+      <c r="C213" t="n">
+        <v>1</v>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>Начал взаимодействие с консультантом!</t>
+        </is>
+      </c>
+      <c r="E213" t="inlineStr">
+        <is>
+          <t>11/06/2023 23:24:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" s="1" t="n">
+        <v>212</v>
+      </c>
+      <c r="B214" t="n">
+        <v>213</v>
+      </c>
+      <c r="C214" t="n">
+        <v>1</v>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>Начал взаимодействие с консультантом!</t>
+        </is>
+      </c>
+      <c r="E214" t="inlineStr">
+        <is>
+          <t>11/06/2023 23:26:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" s="1" t="n">
+        <v>213</v>
+      </c>
+      <c r="B215" t="n">
+        <v>214</v>
+      </c>
+      <c r="C215" t="n">
+        <v>1</v>
+      </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>Начал взаимодействие с консультантом!</t>
+        </is>
+      </c>
+      <c r="E215" t="inlineStr">
+        <is>
+          <t>11/06/2023 23:34:08</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
added mistake explaining function after wrong answer
</commit_message>
<xml_diff>
--- a/data/database_backup/logs.xlsx
+++ b/data/database_backup/logs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E215"/>
+  <dimension ref="A1:E270"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4949,6 +4949,1161 @@
         </is>
       </c>
     </row>
+    <row r="216">
+      <c r="A216" s="1" t="n">
+        <v>214</v>
+      </c>
+      <c r="B216" t="n">
+        <v>215</v>
+      </c>
+      <c r="C216" t="n">
+        <v>1</v>
+      </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>Начал взаимодействие с консультантом!</t>
+        </is>
+      </c>
+      <c r="E216" t="inlineStr">
+        <is>
+          <t>11/06/2023 17:45:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" s="1" t="n">
+        <v>215</v>
+      </c>
+      <c r="B217" t="n">
+        <v>216</v>
+      </c>
+      <c r="C217" t="n">
+        <v>1</v>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>Рассказал партнеру о важности тестирования</t>
+        </is>
+      </c>
+      <c r="E217" t="inlineStr">
+        <is>
+          <t>11/06/2023 17:45:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" s="1" t="n">
+        <v>216</v>
+      </c>
+      <c r="B218" t="n">
+        <v>217</v>
+      </c>
+      <c r="C218" t="n">
+        <v>2</v>
+      </c>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>Начал взаимодействие с консультантом!</t>
+        </is>
+      </c>
+      <c r="E218" t="inlineStr">
+        <is>
+          <t>11/06/2023 17:56:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" s="1" t="n">
+        <v>217</v>
+      </c>
+      <c r="B219" t="n">
+        <v>218</v>
+      </c>
+      <c r="C219" t="n">
+        <v>3</v>
+      </c>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>Начал взаимодействие с консультантом!</t>
+        </is>
+      </c>
+      <c r="E219" t="inlineStr">
+        <is>
+          <t>12/06/2023 06:34:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" s="1" t="n">
+        <v>218</v>
+      </c>
+      <c r="B220" t="n">
+        <v>219</v>
+      </c>
+      <c r="C220" t="n">
+        <v>3</v>
+      </c>
+      <c r="D220" t="inlineStr">
+        <is>
+          <t>Начал тест: sogi_assessment</t>
+        </is>
+      </c>
+      <c r="E220" t="inlineStr">
+        <is>
+          <t>12/06/2023 06:49:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" s="1" t="n">
+        <v>219</v>
+      </c>
+      <c r="B221" t="n">
+        <v>220</v>
+      </c>
+      <c r="C221" t="n">
+        <v>1</v>
+      </c>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>Начал тест: sogi_assessment</t>
+        </is>
+      </c>
+      <c r="E221" t="inlineStr">
+        <is>
+          <t>12/06/2023 06:49:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" s="1" t="n">
+        <v>220</v>
+      </c>
+      <c r="B222" t="n">
+        <v>221</v>
+      </c>
+      <c r="C222" t="n">
+        <v>3</v>
+      </c>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>Завершил тест sogi_assessment!</t>
+        </is>
+      </c>
+      <c r="E222" t="inlineStr">
+        <is>
+          <t>12/06/2023 06:49:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" s="1" t="n">
+        <v>221</v>
+      </c>
+      <c r="B223" t="n">
+        <v>222</v>
+      </c>
+      <c r="C223" t="n">
+        <v>1</v>
+      </c>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>Завершил тест sogi_assessment!</t>
+        </is>
+      </c>
+      <c r="E223" t="inlineStr">
+        <is>
+          <t>12/06/2023 06:49:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" s="1" t="n">
+        <v>222</v>
+      </c>
+      <c r="B224" t="n">
+        <v>223</v>
+      </c>
+      <c r="C224" t="n">
+        <v>3</v>
+      </c>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>Начал тест: pkp_assessment</t>
+        </is>
+      </c>
+      <c r="E224" t="inlineStr">
+        <is>
+          <t>12/06/2023 06:49:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" s="1" t="n">
+        <v>223</v>
+      </c>
+      <c r="B225" t="n">
+        <v>224</v>
+      </c>
+      <c r="C225" t="n">
+        <v>1</v>
+      </c>
+      <c r="D225" t="inlineStr">
+        <is>
+          <t>Начал тест: hiv_risk_assessment</t>
+        </is>
+      </c>
+      <c r="E225" t="inlineStr">
+        <is>
+          <t>12/06/2023 06:49:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" s="1" t="n">
+        <v>224</v>
+      </c>
+      <c r="B226" t="n">
+        <v>225</v>
+      </c>
+      <c r="C226" t="n">
+        <v>3</v>
+      </c>
+      <c r="D226" t="inlineStr">
+        <is>
+          <t>Завершил тест pkp_assessment!</t>
+        </is>
+      </c>
+      <c r="E226" t="inlineStr">
+        <is>
+          <t>12/06/2023 06:49:52</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" s="1" t="n">
+        <v>225</v>
+      </c>
+      <c r="B227" t="n">
+        <v>226</v>
+      </c>
+      <c r="C227" t="n">
+        <v>1</v>
+      </c>
+      <c r="D227" t="inlineStr">
+        <is>
+          <t>Завершил тест hiv_risk_assessment!</t>
+        </is>
+      </c>
+      <c r="E227" t="inlineStr">
+        <is>
+          <t>12/06/2023 06:50:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" s="1" t="n">
+        <v>226</v>
+      </c>
+      <c r="B228" t="n">
+        <v>227</v>
+      </c>
+      <c r="C228" t="n">
+        <v>1</v>
+      </c>
+      <c r="D228" t="inlineStr">
+        <is>
+          <t>Начал тест: pkp_assessment</t>
+        </is>
+      </c>
+      <c r="E228" t="inlineStr">
+        <is>
+          <t>12/06/2023 06:50:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" s="1" t="n">
+        <v>227</v>
+      </c>
+      <c r="B229" t="n">
+        <v>228</v>
+      </c>
+      <c r="C229" t="n">
+        <v>3</v>
+      </c>
+      <c r="D229" t="inlineStr">
+        <is>
+          <t>Начал тест: understanding_PLHIV_assessment</t>
+        </is>
+      </c>
+      <c r="E229" t="inlineStr">
+        <is>
+          <t>12/06/2023 06:50:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" s="1" t="n">
+        <v>228</v>
+      </c>
+      <c r="B230" t="n">
+        <v>229</v>
+      </c>
+      <c r="C230" t="n">
+        <v>1</v>
+      </c>
+      <c r="D230" t="inlineStr">
+        <is>
+          <t>Завершил тест pkp_assessment!</t>
+        </is>
+      </c>
+      <c r="E230" t="inlineStr">
+        <is>
+          <t>12/06/2023 06:50:51</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" s="1" t="n">
+        <v>229</v>
+      </c>
+      <c r="B231" t="n">
+        <v>230</v>
+      </c>
+      <c r="C231" t="n">
+        <v>1</v>
+      </c>
+      <c r="D231" t="inlineStr">
+        <is>
+          <t>Начал тест: understanding_PLHIV_assessment</t>
+        </is>
+      </c>
+      <c r="E231" t="inlineStr">
+        <is>
+          <t>12/06/2023 06:51:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" s="1" t="n">
+        <v>230</v>
+      </c>
+      <c r="B232" t="n">
+        <v>231</v>
+      </c>
+      <c r="C232" t="n">
+        <v>3</v>
+      </c>
+      <c r="D232" t="inlineStr">
+        <is>
+          <t>Завершил тест understanding_PLHIV_assessment!</t>
+        </is>
+      </c>
+      <c r="E232" t="inlineStr">
+        <is>
+          <t>12/06/2023 06:51:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" s="1" t="n">
+        <v>231</v>
+      </c>
+      <c r="B233" t="n">
+        <v>232</v>
+      </c>
+      <c r="C233" t="n">
+        <v>3</v>
+      </c>
+      <c r="D233" t="inlineStr">
+        <is>
+          <t>Начал тест: hiv_risk_assessment</t>
+        </is>
+      </c>
+      <c r="E233" t="inlineStr">
+        <is>
+          <t>12/06/2023 06:52:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" s="1" t="n">
+        <v>232</v>
+      </c>
+      <c r="B234" t="n">
+        <v>233</v>
+      </c>
+      <c r="C234" t="n">
+        <v>3</v>
+      </c>
+      <c r="D234" t="inlineStr">
+        <is>
+          <t>Завершил тест hiv_risk_assessment!</t>
+        </is>
+      </c>
+      <c r="E234" t="inlineStr">
+        <is>
+          <t>12/06/2023 06:52:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" s="1" t="n">
+        <v>233</v>
+      </c>
+      <c r="B235" t="n">
+        <v>234</v>
+      </c>
+      <c r="C235" t="n">
+        <v>6</v>
+      </c>
+      <c r="D235" t="inlineStr">
+        <is>
+          <t>Успешно добавлен в базу!</t>
+        </is>
+      </c>
+      <c r="E235" t="inlineStr">
+        <is>
+          <t>12/06/2023 07:07:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" s="1" t="n">
+        <v>234</v>
+      </c>
+      <c r="B236" t="n">
+        <v>235</v>
+      </c>
+      <c r="C236" t="n">
+        <v>1</v>
+      </c>
+      <c r="D236" t="inlineStr">
+        <is>
+          <t>Начал взаимодействие с консультантом!</t>
+        </is>
+      </c>
+      <c r="E236" t="inlineStr">
+        <is>
+          <t>12/06/2023 07:20:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" s="1" t="n">
+        <v>235</v>
+      </c>
+      <c r="B237" t="n">
+        <v>236</v>
+      </c>
+      <c r="C237" t="n">
+        <v>1</v>
+      </c>
+      <c r="D237" t="inlineStr">
+        <is>
+          <t>Попытался заказать тест на ВИЧ!</t>
+        </is>
+      </c>
+      <c r="E237" t="inlineStr">
+        <is>
+          <t>12/06/2023 07:20:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" s="1" t="n">
+        <v>236</v>
+      </c>
+      <c r="B238" t="n">
+        <v>237</v>
+      </c>
+      <c r="C238" t="n">
+        <v>1</v>
+      </c>
+      <c r="D238" t="inlineStr">
+        <is>
+          <t>Начал тест: hiv_knowledge_assessment</t>
+        </is>
+      </c>
+      <c r="E238" t="inlineStr">
+        <is>
+          <t>12/06/2023 07:20:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" s="1" t="n">
+        <v>237</v>
+      </c>
+      <c r="B239" t="n">
+        <v>238</v>
+      </c>
+      <c r="C239" t="n">
+        <v>1</v>
+      </c>
+      <c r="D239" t="inlineStr">
+        <is>
+          <t>Попытался заказать тест на ВИЧ!</t>
+        </is>
+      </c>
+      <c r="E239" t="inlineStr">
+        <is>
+          <t>12/06/2023 07:20:58</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" s="1" t="n">
+        <v>238</v>
+      </c>
+      <c r="B240" t="n">
+        <v>239</v>
+      </c>
+      <c r="C240" t="n">
+        <v>1</v>
+      </c>
+      <c r="D240" t="inlineStr">
+        <is>
+          <t>Начал взаимодействие с консультантом!</t>
+        </is>
+      </c>
+      <c r="E240" t="inlineStr">
+        <is>
+          <t>12/06/2023 07:21:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" s="1" t="n">
+        <v>239</v>
+      </c>
+      <c r="B241" t="n">
+        <v>240</v>
+      </c>
+      <c r="C241" t="n">
+        <v>6</v>
+      </c>
+      <c r="D241" t="inlineStr">
+        <is>
+          <t>Начал взаимодействие с консультантом!</t>
+        </is>
+      </c>
+      <c r="E241" t="inlineStr">
+        <is>
+          <t>12/06/2023 07:21:58</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" s="1" t="n">
+        <v>240</v>
+      </c>
+      <c r="B242" t="n">
+        <v>241</v>
+      </c>
+      <c r="C242" t="n">
+        <v>1</v>
+      </c>
+      <c r="D242" t="inlineStr">
+        <is>
+          <t>Успешно добавлен в базу!</t>
+        </is>
+      </c>
+      <c r="E242" t="inlineStr">
+        <is>
+          <t>12/06/2023 07:42:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" s="1" t="n">
+        <v>241</v>
+      </c>
+      <c r="B243" t="n">
+        <v>242</v>
+      </c>
+      <c r="C243" t="n">
+        <v>1</v>
+      </c>
+      <c r="D243" t="inlineStr">
+        <is>
+          <t>Начал тест: pkp_assessment</t>
+        </is>
+      </c>
+      <c r="E243" t="inlineStr">
+        <is>
+          <t>16/06/2023 14:42:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" s="1" t="n">
+        <v>242</v>
+      </c>
+      <c r="B244" t="n">
+        <v>243</v>
+      </c>
+      <c r="C244" t="n">
+        <v>1</v>
+      </c>
+      <c r="D244" t="inlineStr">
+        <is>
+          <t>Начал тест: pkp_assessment</t>
+        </is>
+      </c>
+      <c r="E244" t="inlineStr">
+        <is>
+          <t>16/06/2023 14:44:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" s="1" t="n">
+        <v>243</v>
+      </c>
+      <c r="B245" t="n">
+        <v>244</v>
+      </c>
+      <c r="C245" t="n">
+        <v>1</v>
+      </c>
+      <c r="D245" t="inlineStr">
+        <is>
+          <t>Начал тест: pkp_assessment</t>
+        </is>
+      </c>
+      <c r="E245" t="inlineStr">
+        <is>
+          <t>16/06/2023 15:20:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" s="1" t="n">
+        <v>244</v>
+      </c>
+      <c r="B246" t="n">
+        <v>245</v>
+      </c>
+      <c r="C246" t="n">
+        <v>1</v>
+      </c>
+      <c r="D246" t="inlineStr">
+        <is>
+          <t>Завершил тест pkp_assessment!</t>
+        </is>
+      </c>
+      <c r="E246" t="inlineStr">
+        <is>
+          <t>16/06/2023 15:24:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" s="1" t="n">
+        <v>245</v>
+      </c>
+      <c r="B247" t="n">
+        <v>246</v>
+      </c>
+      <c r="C247" t="n">
+        <v>1</v>
+      </c>
+      <c r="D247" t="inlineStr">
+        <is>
+          <t>Начал тест: hiv_knowledge_assessment</t>
+        </is>
+      </c>
+      <c r="E247" t="inlineStr">
+        <is>
+          <t>16/06/2023 15:26:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" s="1" t="n">
+        <v>246</v>
+      </c>
+      <c r="B248" t="n">
+        <v>247</v>
+      </c>
+      <c r="C248" t="n">
+        <v>1</v>
+      </c>
+      <c r="D248" t="inlineStr">
+        <is>
+          <t>Начал тест: sogi_assessment</t>
+        </is>
+      </c>
+      <c r="E248" t="inlineStr">
+        <is>
+          <t>16/06/2023 15:27:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" s="1" t="n">
+        <v>247</v>
+      </c>
+      <c r="B249" t="n">
+        <v>248</v>
+      </c>
+      <c r="C249" t="n">
+        <v>1</v>
+      </c>
+      <c r="D249" t="inlineStr">
+        <is>
+          <t>Начал тест: sogi_assessment</t>
+        </is>
+      </c>
+      <c r="E249" t="inlineStr">
+        <is>
+          <t>16/06/2023 15:31:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" s="1" t="n">
+        <v>248</v>
+      </c>
+      <c r="B250" t="n">
+        <v>249</v>
+      </c>
+      <c r="C250" t="n">
+        <v>1</v>
+      </c>
+      <c r="D250" t="inlineStr">
+        <is>
+          <t>Начал тест: sogi_assessment</t>
+        </is>
+      </c>
+      <c r="E250" t="inlineStr">
+        <is>
+          <t>16/06/2023 15:32:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" s="1" t="n">
+        <v>249</v>
+      </c>
+      <c r="B251" t="n">
+        <v>250</v>
+      </c>
+      <c r="C251" t="n">
+        <v>1</v>
+      </c>
+      <c r="D251" t="inlineStr">
+        <is>
+          <t>Начал тест: pkp_assessment</t>
+        </is>
+      </c>
+      <c r="E251" t="inlineStr">
+        <is>
+          <t>16/06/2023 15:36:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" s="1" t="n">
+        <v>250</v>
+      </c>
+      <c r="B252" t="n">
+        <v>251</v>
+      </c>
+      <c r="C252" t="n">
+        <v>1</v>
+      </c>
+      <c r="D252" t="inlineStr">
+        <is>
+          <t>Начал тест: hiv_risk_assessment</t>
+        </is>
+      </c>
+      <c r="E252" t="inlineStr">
+        <is>
+          <t>16/06/2023 15:36:46</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" s="1" t="n">
+        <v>251</v>
+      </c>
+      <c r="B253" t="n">
+        <v>252</v>
+      </c>
+      <c r="C253" t="n">
+        <v>1</v>
+      </c>
+      <c r="D253" t="inlineStr">
+        <is>
+          <t>Начал тест: hiv_risk_assessment</t>
+        </is>
+      </c>
+      <c r="E253" t="inlineStr">
+        <is>
+          <t>16/06/2023 16:07:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" s="1" t="n">
+        <v>252</v>
+      </c>
+      <c r="B254" t="n">
+        <v>253</v>
+      </c>
+      <c r="C254" t="n">
+        <v>1</v>
+      </c>
+      <c r="D254" t="inlineStr">
+        <is>
+          <t>Завершил тест hiv_risk_assessment!</t>
+        </is>
+      </c>
+      <c r="E254" t="inlineStr">
+        <is>
+          <t>16/06/2023 16:07:58</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" s="1" t="n">
+        <v>253</v>
+      </c>
+      <c r="B255" t="n">
+        <v>254</v>
+      </c>
+      <c r="C255" t="n">
+        <v>1</v>
+      </c>
+      <c r="D255" t="inlineStr">
+        <is>
+          <t>Начал тест: sogi_assessment</t>
+        </is>
+      </c>
+      <c r="E255" t="inlineStr">
+        <is>
+          <t>16/06/2023 16:08:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" s="1" t="n">
+        <v>254</v>
+      </c>
+      <c r="B256" t="n">
+        <v>255</v>
+      </c>
+      <c r="C256" t="n">
+        <v>1</v>
+      </c>
+      <c r="D256" t="inlineStr">
+        <is>
+          <t>Начал тест: pkp_assessment</t>
+        </is>
+      </c>
+      <c r="E256" t="inlineStr">
+        <is>
+          <t>16/06/2023 16:09:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" s="1" t="n">
+        <v>255</v>
+      </c>
+      <c r="B257" t="n">
+        <v>256</v>
+      </c>
+      <c r="C257" t="n">
+        <v>1</v>
+      </c>
+      <c r="D257" t="inlineStr">
+        <is>
+          <t>Завершил тест pkp_assessment!</t>
+        </is>
+      </c>
+      <c r="E257" t="inlineStr">
+        <is>
+          <t>16/06/2023 16:10:25</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" s="1" t="n">
+        <v>256</v>
+      </c>
+      <c r="B258" t="n">
+        <v>257</v>
+      </c>
+      <c r="C258" t="n">
+        <v>1</v>
+      </c>
+      <c r="D258" t="inlineStr">
+        <is>
+          <t>Начал тест: pkp_assessment</t>
+        </is>
+      </c>
+      <c r="E258" t="inlineStr">
+        <is>
+          <t>16/06/2023 16:11:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" s="1" t="n">
+        <v>257</v>
+      </c>
+      <c r="B259" t="n">
+        <v>258</v>
+      </c>
+      <c r="C259" t="n">
+        <v>1</v>
+      </c>
+      <c r="D259" t="inlineStr">
+        <is>
+          <t>Завершил тест pkp_assessment!</t>
+        </is>
+      </c>
+      <c r="E259" t="inlineStr">
+        <is>
+          <t>16/06/2023 16:12:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" s="1" t="n">
+        <v>258</v>
+      </c>
+      <c r="B260" t="n">
+        <v>259</v>
+      </c>
+      <c r="C260" t="n">
+        <v>1</v>
+      </c>
+      <c r="D260" t="inlineStr">
+        <is>
+          <t>Начал тест: sogi_assessment</t>
+        </is>
+      </c>
+      <c r="E260" t="inlineStr">
+        <is>
+          <t>16/06/2023 16:29:18</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" s="1" t="n">
+        <v>259</v>
+      </c>
+      <c r="B261" t="n">
+        <v>260</v>
+      </c>
+      <c r="C261" t="n">
+        <v>1</v>
+      </c>
+      <c r="D261" t="inlineStr">
+        <is>
+          <t>Начал тест: sogi_assessment</t>
+        </is>
+      </c>
+      <c r="E261" t="inlineStr">
+        <is>
+          <t>16/06/2023 16:30:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" s="1" t="n">
+        <v>260</v>
+      </c>
+      <c r="B262" t="n">
+        <v>261</v>
+      </c>
+      <c r="C262" t="n">
+        <v>1</v>
+      </c>
+      <c r="D262" t="inlineStr">
+        <is>
+          <t>Завершил тест sogi_assessment!</t>
+        </is>
+      </c>
+      <c r="E262" t="inlineStr">
+        <is>
+          <t>16/06/2023 16:31:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" s="1" t="n">
+        <v>261</v>
+      </c>
+      <c r="B263" t="n">
+        <v>262</v>
+      </c>
+      <c r="C263" t="n">
+        <v>1</v>
+      </c>
+      <c r="D263" t="inlineStr">
+        <is>
+          <t>Начал тест: sogi_assessment</t>
+        </is>
+      </c>
+      <c r="E263" t="inlineStr">
+        <is>
+          <t>16/06/2023 17:57:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" s="1" t="n">
+        <v>262</v>
+      </c>
+      <c r="B264" t="n">
+        <v>263</v>
+      </c>
+      <c r="C264" t="n">
+        <v>1</v>
+      </c>
+      <c r="D264" t="inlineStr">
+        <is>
+          <t>Начал тест: sogi_assessment</t>
+        </is>
+      </c>
+      <c r="E264" t="inlineStr">
+        <is>
+          <t>16/06/2023 17:59:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" s="1" t="n">
+        <v>263</v>
+      </c>
+      <c r="B265" t="n">
+        <v>264</v>
+      </c>
+      <c r="C265" t="n">
+        <v>1</v>
+      </c>
+      <c r="D265" t="inlineStr">
+        <is>
+          <t>Начал тест: sogi_assessment</t>
+        </is>
+      </c>
+      <c r="E265" t="inlineStr">
+        <is>
+          <t>16/06/2023 18:00:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" s="1" t="n">
+        <v>264</v>
+      </c>
+      <c r="B266" t="n">
+        <v>265</v>
+      </c>
+      <c r="C266" t="n">
+        <v>1</v>
+      </c>
+      <c r="D266" t="inlineStr">
+        <is>
+          <t>Завершил тест sogi_assessment!</t>
+        </is>
+      </c>
+      <c r="E266" t="inlineStr">
+        <is>
+          <t>16/06/2023 18:02:52</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" s="1" t="n">
+        <v>265</v>
+      </c>
+      <c r="B267" t="n">
+        <v>266</v>
+      </c>
+      <c r="C267" t="n">
+        <v>1</v>
+      </c>
+      <c r="D267" t="inlineStr">
+        <is>
+          <t>Начал тест: sogi_assessment</t>
+        </is>
+      </c>
+      <c r="E267" t="inlineStr">
+        <is>
+          <t>16/06/2023 18:03:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" s="1" t="n">
+        <v>266</v>
+      </c>
+      <c r="B268" t="n">
+        <v>267</v>
+      </c>
+      <c r="C268" t="n">
+        <v>1</v>
+      </c>
+      <c r="D268" t="inlineStr">
+        <is>
+          <t>Завершил тест sogi_assessment!</t>
+        </is>
+      </c>
+      <c r="E268" t="inlineStr">
+        <is>
+          <t>16/06/2023 18:04:25</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" s="1" t="n">
+        <v>267</v>
+      </c>
+      <c r="B269" t="n">
+        <v>268</v>
+      </c>
+      <c r="C269" t="n">
+        <v>1</v>
+      </c>
+      <c r="D269" t="inlineStr">
+        <is>
+          <t>Начал тест: hiv_risk_assessment</t>
+        </is>
+      </c>
+      <c r="E269" t="inlineStr">
+        <is>
+          <t>16/06/2023 18:04:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" s="1" t="n">
+        <v>268</v>
+      </c>
+      <c r="B270" t="n">
+        <v>269</v>
+      </c>
+      <c r="C270" t="n">
+        <v>1</v>
+      </c>
+      <c r="D270" t="inlineStr">
+        <is>
+          <t>Завершил тест hiv_risk_assessment!</t>
+        </is>
+      </c>
+      <c r="E270" t="inlineStr">
+        <is>
+          <t>16/06/2023 18:05:25</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
added tools to set | modify | delete personal reminders user will be able to set reminder about his drug on specific time ('h:m' format ony)
</commit_message>
<xml_diff>
--- a/data/database_backup/logs.xlsx
+++ b/data/database_backup/logs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -560,6 +560,48 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>6</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Начал взаимодействие с консультантом!</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>11/11/2023 11:50:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>7</v>
+      </c>
+      <c r="C8" t="n">
+        <v>3</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Успешно добавлен в базу!</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>11/11/2023 16:08:54</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
added taking meds history viewing function
</commit_message>
<xml_diff>
--- a/data/database_backup/logs.xlsx
+++ b/data/database_backup/logs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -602,6 +602,27 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>9</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2023-11-22 | Jan:01 - препарат принят (От поноса)</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>22/11/2023 20:09:39</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
I hope this was the last bug T_T
</commit_message>
<xml_diff>
--- a/data/database_backup/logs.xlsx
+++ b/data/database_backup/logs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -623,6 +623,49 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>10</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2023-11-22 | 14:14 - препарат принят (таблетки)</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>22/11/2023 14:42:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>11</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2023-11-22 | 21:21 - препарат принят ( 1234
+)</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>22/11/2023 21:00:13</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>